<commit_message>
dialog 검수 1차 끝
줄바꿈 관련 문제 생길 수 있음
</commit_message>
<xml_diff>
--- a/Mod_Korean/Lang/KR/Dialog/Drama/casino_clerk.xlsx
+++ b/Mod_Korean/Lang/KR/Dialog/Drama/casino_clerk.xlsx
@@ -2,25 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr autoCompressPictures="1"/>
-  <workbookProtection lockStructure="0" lockWindows="0" lockRevision="0"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="16384" windowHeight="8192" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" r:id="rId3"/>
+    <sheet name="1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001" fullPrecision="1" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
-    <ext uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr xmlns:loext="http://schemas.libreoffice.org/" stringRefSyntax="CalcA1"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t xml:space="preserve">step</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">This is your first visit today, yes? Here is your free scratch card! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">오늘 처음 방문하신 {거냐}? 여기 스크래치 카드{다}!</t>
   </si>
   <si>
     <t xml:space="preserve">invoke</t>
@@ -143,7 +146,7 @@
     <t xml:space="preserve">The golden bell heralds good fortune... Welcome to the 'Fortune Bell,' the world's only casino airship. Feel free to enjoy until your wallet is empty.</t>
   </si>
   <si>
-    <t xml:space="preserve">#guild欢迎回来，#pc。你现在的等级是#guild_title{语尾}。今天有什么事{语尾}？</t>
+    <t xml:space="preserve">황금의 종이 행운을 고한다… 세상의 유일무이한 카지노, 비공정 「포츈 벨」에 어서 {와}! 지갑이 텅텅 비게 될 때까지 안심하고 즐겨 {줘}.</t>
   </si>
   <si>
     <t xml:space="preserve">inject</t>
@@ -156,15 +159,6 @@
   </si>
   <si>
     <t xml:space="preserve">cancel</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">처음 방문하신 {거냐}? 여기 스크래치 카드{다}!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">황금의 종이, 행운을 고한다… 세상의 유일무이한 카지노, 비공정 「포츈 벨」에 어서 {와}! 지갑이 텅텅 비게 될 때까지 안심하고 즐겨 {줘}.</t>
   </si>
 </sst>
 </file>
@@ -186,20 +180,20 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family/>
-      <charset val="128"/>
+      <family val="0"/>
+      <charset val="129"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family/>
-      <charset val="128"/>
+      <family val="0"/>
+      <charset val="129"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family/>
-      <charset val="128"/>
+      <family val="0"/>
+      <charset val="129"/>
     </font>
     <font>
       <sz val="10"/>
@@ -231,7 +225,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -240,54 +234,54 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection locked="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0">
-      <alignment/>
-      <protection locked="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection locked="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection locked="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection locked="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection locked="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection locked="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -301,13 +295,13 @@
   <dxfs count="1">
     <dxf>
       <font>
+        <name val="游ゴシック"/>
+        <charset val="128"/>
+        <family val="2"/>
         <color rgb="FFCC0000"/>
-        <name val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill>
           <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
@@ -483,32 +477,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="L14" sqref="L14"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="8.85" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.56" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85" style="1" customWidth="1"/>
-    <col min="8" max="9" width="7.09" style="1" customWidth="1"/>
-    <col min="10" max="10" width="42.14" style="1" customWidth="1"/>
-    <col min="11" max="11" width="53.28" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="7.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="42.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="53.28"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,28 +540,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="12.8">
-      <c r="I2" s="1">
-        <f>MAX(I4:I1048576)</f>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="1" t="n">
+        <f aca="false">MAX(I4:I1048576)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="12.8">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="12.8">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="12.8">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" ht="12.8">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -575,8 +569,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="12.8">
-      <c r="I10" s="1">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -585,69 +579,69 @@
       <c r="K10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" ht="12.8">
+      <c r="L10" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" ht="12.8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" ht="12.8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" ht="14.15">
-      <c r="I14" s="1">
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" ht="12.8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" ht="12.8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" ht="12.8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4:I1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>

</xml_diff>